<commit_message>
Gathered and applied new phase weights.
</commit_message>
<xml_diff>
--- a/DupFileFinder/PhaseWeightCalculator.xlsx
+++ b/DupFileFinder/PhaseWeightCalculator.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C92E2B-C3D8-466E-989C-0D0A78B6E1C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643C4F5B-138E-489F-AB86-F8FD7A88617F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6810" yWindow="2880" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7020" yWindow="630" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
   <si>
     <t>Phase</t>
   </si>
@@ -75,7 +75,34 @@
     <t>on</t>
   </si>
   <si>
-    <t>Done on D:\. Below is bogus because program had just been run</t>
+    <t>These tests are to be done against the roots of all 3 of the drives on my pc, immediately following reboots.</t>
+  </si>
+  <si>
+    <t>Found</t>
+  </si>
+  <si>
+    <t>bytes in</t>
+  </si>
+  <si>
+    <t>redundant files</t>
+  </si>
+  <si>
+    <t>percent of the time required for the other option</t>
+  </si>
+  <si>
+    <t>There were some files added/removed/or changed between these tests.</t>
+  </si>
+  <si>
+    <t>Test Date:</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>Because the difference in results (less than 0.3%) is small, comparisons are adequate.</t>
+  </si>
+  <si>
+    <t>Interesting how much less time was required when the Checksum was turned off.</t>
   </si>
 </sst>
 </file>
@@ -119,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -128,6 +155,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,326 +507,466 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" customWidth="1"/>
     <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="2"/>
+      <c r="B1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="7">
+        <v>44547</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="6"/>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>31</v>
-      </c>
-      <c r="H2">
-        <f xml:space="preserve"> G2 + 1000 * (F2 + 60 * (E2 + 60 * (D2 + 24 * C2)))</f>
-        <v>1031</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>441</v>
-      </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H12" si="0" xml:space="preserve"> G3 + 1000 * (F3 + 60 * (E3 + 60 * (D3 + 24 * C3)))</f>
-        <v>441</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-      <c r="G5">
-        <v>949</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="0"/>
-        <v>2949</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>178</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="0"/>
-        <v>1178</v>
-      </c>
-      <c r="I6">
-        <f>SUM(H2:H6)</f>
-        <v>5599</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>969</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="0"/>
-        <v>969</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>471</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="0"/>
-        <v>471</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C9" s="9">
+        <v>0</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="9">
+        <v>41</v>
+      </c>
+      <c r="G9" s="9">
+        <v>398</v>
+      </c>
+      <c r="H9" s="9">
+        <f xml:space="preserve"> G9 + 1000 * (F9 + 60 * (E9 + 60 * (D9 + 24 * C9)))</f>
+        <v>101398</v>
+      </c>
+      <c r="I9" s="9"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>2</v>
-      </c>
-      <c r="G10">
-        <v>633</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="0"/>
-        <v>2633</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C10" s="9">
+        <v>0</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0</v>
+      </c>
+      <c r="F10" s="9">
+        <v>49</v>
+      </c>
+      <c r="G10" s="9">
+        <v>371</v>
+      </c>
+      <c r="H10" s="9">
+        <f t="shared" ref="H10:H21" si="0" xml:space="preserve"> G10 + 1000 * (F10 + 60 * (E10 + 60 * (D10 + 24 * C10)))</f>
+        <v>49371</v>
+      </c>
+      <c r="I10" s="9"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>330</v>
-      </c>
-      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0</v>
+      </c>
+      <c r="E11" s="9">
+        <v>0</v>
+      </c>
+      <c r="F11" s="9">
+        <v>0</v>
+      </c>
+      <c r="G11" s="9">
+        <v>0</v>
+      </c>
+      <c r="H11" s="9">
         <f t="shared" si="0"/>
-        <v>1330</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I11" s="9"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="9">
+        <v>0</v>
+      </c>
+      <c r="D12" s="9">
+        <v>2</v>
+      </c>
+      <c r="E12" s="9">
+        <v>4</v>
+      </c>
+      <c r="F12" s="9">
+        <v>34</v>
+      </c>
+      <c r="G12" s="9">
+        <v>932</v>
+      </c>
+      <c r="H12" s="9">
+        <f t="shared" si="0"/>
+        <v>7474932</v>
+      </c>
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0</v>
+      </c>
+      <c r="E13" s="9">
+        <v>25</v>
+      </c>
+      <c r="F13" s="9">
+        <v>59</v>
+      </c>
+      <c r="G13" s="9">
+        <v>964</v>
+      </c>
+      <c r="H13" s="9">
+        <f t="shared" si="0"/>
+        <v>1559964</v>
+      </c>
+      <c r="I13" s="9">
+        <f>SUM(H9:H13)</f>
+        <v>9185665</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="5">
+        <v>132597599496</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="5">
+        <v>219604</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f>100*I13/I21</f>
+        <v>27.623763016398787</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>23</v>
+      </c>
+      <c r="G17">
+        <v>319</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>83319</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>39</v>
+      </c>
+      <c r="G18">
+        <v>155</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>39155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>33</v>
+      </c>
+      <c r="F19">
+        <v>10</v>
+      </c>
+      <c r="G19">
+        <v>507</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>12790507</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <v>17</v>
+      </c>
+      <c r="F20">
+        <v>43</v>
+      </c>
+      <c r="G20">
+        <v>682</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>19063682</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>21</v>
+      </c>
+      <c r="F21">
+        <v>16</v>
+      </c>
+      <c r="G21">
+        <v>102</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>1276102</v>
+      </c>
+      <c r="I21">
+        <f>SUM(H17:H21)</f>
+        <v>33252765</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="5">
+        <v>132563600853</v>
+      </c>
+      <c r="C22" t="s">
         <v>17</v>
       </c>
-      <c r="G12">
-        <v>539</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="0"/>
-        <v>17539</v>
-      </c>
-      <c r="I12">
-        <f>SUM(H8:H12)</f>
-        <v>22942</v>
+      <c r="D22" s="5">
+        <v>220234</v>
+      </c>
+      <c r="E22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f>100*I21/I13</f>
+        <v>362.00716006952138</v>
+      </c>
+      <c r="B23" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>